<commit_message>
Update: Ensure Midlothian dashboard has all latest features and fixes
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-Midlothian/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA9D059-6D31-9042-BA11-5544D450B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4010B267-6F94-AC41-A5A3-CEBFB3F99B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="760" windowWidth="23740" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="8500" windowWidth="28140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update source file with user changes
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{421B1B56-588C-1D4D-A00C-592804088268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F2F5AF-02DE-1943-A508-BBA78B5194F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="6340" windowWidth="26440" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$86</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -553,12 +556,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -588,11 +597,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,11 +907,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AE93" sqref="AE93"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="21" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="35" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1061,7 +1125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1371,7 +1435,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1526,7 +1590,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1678,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1830,159 +1894,159 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:52" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="s">
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AA7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE7" t="s">
+      <c r="AA7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
+      <c r="AF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="2">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AH7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AI7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ7">
+      <c r="AI7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ7" s="2">
         <v>29</v>
       </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <v>0</v>
-      </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
-      <c r="AP7">
+      <c r="AK7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="2">
         <v>67</v>
       </c>
-      <c r="AQ7">
-        <v>0</v>
-      </c>
-      <c r="AR7">
-        <v>0</v>
-      </c>
-      <c r="AS7">
-        <v>0</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="AU7">
-        <v>0</v>
-      </c>
-      <c r="AV7">
-        <v>0</v>
-      </c>
-      <c r="AW7">
-        <v>0</v>
-      </c>
-      <c r="AX7">
-        <v>0</v>
-      </c>
-      <c r="AY7">
-        <v>0</v>
-      </c>
-      <c r="AZ7">
+      <c r="AQ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2137,7 +2201,7 @@
         <v>83.333333333333343</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2295,7 +2359,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2450,7 +2514,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2605,7 +2669,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2760,7 +2824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -2915,7 +2979,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -3070,7 +3134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -3222,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -3377,8 +3441,8 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B17">
@@ -3532,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3684,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -3839,7 +3903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -3994,7 +4058,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -4149,7 +4213,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -4304,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -4459,7 +4523,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -4614,7 +4678,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -4769,8 +4833,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B26">
@@ -4924,7 +4988,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -5079,7 +5143,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -5234,7 +5298,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -5389,7 +5453,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -5544,7 +5608,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -5699,7 +5763,7 @@
         <v>83.333333333333343</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -5854,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -6009,7 +6073,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -6164,7 +6228,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -6316,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -6471,7 +6535,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -6626,8 +6690,8 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B38">
@@ -6781,7 +6845,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -6936,7 +7000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -7091,7 +7155,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -7243,7 +7307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -7398,8 +7462,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B43">
@@ -7553,7 +7617,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -7708,7 +7772,7 @@
         <v>83.333333333333343</v>
       </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -7863,7 +7927,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -8107,7 +8171,7 @@
         <v>159</v>
       </c>
       <c r="AE47" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF47">
         <v>232.0196428571428</v>
@@ -8173,7 +8237,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -8328,7 +8392,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -8480,7 +8544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -8632,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -8787,7 +8851,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -8942,7 +9006,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -9097,7 +9161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -9252,7 +9316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -9407,7 +9471,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -9559,7 +9623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -9714,7 +9778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -9869,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -10024,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -10176,7 +10240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -10331,7 +10395,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -10489,7 +10553,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>113</v>
       </c>
@@ -10644,7 +10708,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>114</v>
       </c>
@@ -10799,7 +10863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>115</v>
       </c>
@@ -10951,7 +11015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -11106,7 +11170,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>117</v>
       </c>
@@ -11258,7 +11322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>118</v>
       </c>
@@ -11410,7 +11474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>119</v>
       </c>
@@ -11562,7 +11626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>120</v>
       </c>
@@ -11714,7 +11778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>121</v>
       </c>
@@ -11869,7 +11933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>122</v>
       </c>
@@ -12027,8 +12091,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B73">
@@ -12182,7 +12246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>124</v>
       </c>
@@ -12337,7 +12401,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>125</v>
       </c>
@@ -12492,7 +12556,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>126</v>
       </c>
@@ -12644,7 +12708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>127</v>
       </c>
@@ -12799,7 +12863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -12954,7 +13018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -13109,7 +13173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>130</v>
       </c>
@@ -13264,7 +13328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>131</v>
       </c>
@@ -13416,7 +13480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>132</v>
       </c>
@@ -13571,7 +13635,7 @@
         <v>16.666666666666661</v>
       </c>
     </row>
-    <row r="83" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>133</v>
       </c>
@@ -13723,7 +13787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>134</v>
       </c>
@@ -13878,7 +13942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>135</v>
       </c>
@@ -14033,7 +14097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>136</v>
       </c>
@@ -14189,6 +14253,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AZ86" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="614200 Internet &amp; Social media"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update expense-analysis.xlsx source file with latest data
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F2F5AF-02DE-1943-A508-BBA78B5194F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F39B3741-DC44-7949-A66F-4796F83ECA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="6340" windowWidth="26440" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="760" windowWidth="25360" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,13 +172,13 @@
     <t>Total Excess Costs (5% Buffer)</t>
   </si>
   <si>
-    <t>% of Months Outpaced Growth</t>
-  </si>
-  <si>
-    <t>% of Months Did Not Decline with Profit</t>
-  </si>
-  <si>
-    <t>% of Months Opposite Direction than Profit</t>
+    <t># of Months Outpaced Growth</t>
+  </si>
+  <si>
+    <t># of Months Did Not Decline with Profit</t>
+  </si>
+  <si>
+    <t># of Months Opposite Direction than Profit</t>
   </si>
   <si>
     <t xml:space="preserve">   400000 Management Fees</t>
@@ -907,11 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AZ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE93" sqref="AE93"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AY1" sqref="AY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -962,9 +961,9 @@
     <col min="47" max="47" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="25" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.2">
@@ -1125,7 +1124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1426,16 +1425,16 @@
         <v>398.27981777279672</v>
       </c>
       <c r="AX3">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY3">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ3">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1581,16 +1580,16 @@
         <v>915.76569624870388</v>
       </c>
       <c r="AX4">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY4">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ4">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1733,16 +1732,16 @@
         <v>0</v>
       </c>
       <c r="AX5">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY5">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1894,159 +1893,159 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:52" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
         <v>138</v>
       </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
         <v>145</v>
       </c>
-      <c r="AA7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AA7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE7" t="s">
         <v>162</v>
       </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="2">
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AH7" t="s">
         <v>166</v>
       </c>
-      <c r="AI7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ7" s="2">
+      <c r="AI7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ7">
         <v>29</v>
       </c>
-      <c r="AK7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="2">
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
         <v>67</v>
       </c>
-      <c r="AQ7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="2">
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2192,16 +2191,16 @@
         <v>12332.34393450957</v>
       </c>
       <c r="AX8">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY8">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ8">
-        <v>83.333333333333343</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2350,16 +2349,16 @@
         <v>3367.4322113797061</v>
       </c>
       <c r="AX9">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY9">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ9">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2505,16 +2504,16 @@
         <v>8924.4517453896242</v>
       </c>
       <c r="AX10">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY10">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ10">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2660,16 +2659,16 @@
         <v>5530.5817263010131</v>
       </c>
       <c r="AX11">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY11">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ11">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2815,16 +2814,16 @@
         <v>2521.1125907723372</v>
       </c>
       <c r="AX12">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY12">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ12">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -2970,16 +2969,16 @@
         <v>722.87408227344599</v>
       </c>
       <c r="AX13">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY13">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ13">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -3125,16 +3124,16 @@
         <v>33283.022545252767</v>
       </c>
       <c r="AX14">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY14">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ14">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -3432,17 +3431,17 @@
         <v>13996.88007225446</v>
       </c>
       <c r="AX16">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY16">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ16">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>67</v>
       </c>
       <c r="B17">
@@ -3587,16 +3586,16 @@
         <v>3281.37</v>
       </c>
       <c r="AX17">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY17">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3739,16 +3738,16 @@
         <v>519.22</v>
       </c>
       <c r="AX18">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY18">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -3894,16 +3893,16 @@
         <v>15602.500072254459</v>
       </c>
       <c r="AX19">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY19">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ19">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -4049,16 +4048,16 @@
         <v>9269.0867138464</v>
       </c>
       <c r="AX20">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY20">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ20">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -4204,16 +4203,16 @@
         <v>210.76528876877529</v>
       </c>
       <c r="AX21">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY21">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ21">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -4359,16 +4358,16 @@
         <v>395.77532672975639</v>
       </c>
       <c r="AX22">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY22">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -4514,16 +4513,16 @@
         <v>554.03902380088778</v>
       </c>
       <c r="AX23">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY23">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ23">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -4669,16 +4668,16 @@
         <v>157.1338204411293</v>
       </c>
       <c r="AX24">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY24">
         <v>0</v>
       </c>
       <c r="AZ24">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -4824,17 +4823,17 @@
         <v>109.5310421034078</v>
       </c>
       <c r="AX25">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY25">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>76</v>
       </c>
       <c r="B26">
@@ -4979,16 +4978,16 @@
         <v>2846.8977307856371</v>
       </c>
       <c r="AX26">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY26">
         <v>0</v>
       </c>
       <c r="AZ26">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -5134,16 +5133,16 @@
         <v>1035.0390149343521</v>
       </c>
       <c r="AX27">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY27">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ27">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -5289,16 +5288,16 @@
         <v>564.8062234999154</v>
       </c>
       <c r="AX28">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY28">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ28">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -5444,16 +5443,16 @@
         <v>2158.8170182416588</v>
       </c>
       <c r="AX29">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY29">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ29">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -5599,16 +5598,16 @@
         <v>1514.4434244594979</v>
       </c>
       <c r="AX30">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY30">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ30">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -5754,16 +5753,16 @@
         <v>3647.8962162012949</v>
       </c>
       <c r="AX31">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY31">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ31">
-        <v>83.333333333333343</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -5918,7 +5917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -6064,16 +6063,16 @@
         <v>838.55</v>
       </c>
       <c r="AX33">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY33">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ33">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -6219,16 +6218,16 @@
         <v>346.97</v>
       </c>
       <c r="AX34">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY34">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ34">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -6380,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -6526,16 +6525,16 @@
         <v>4642.5880210794458</v>
       </c>
       <c r="AX36">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY36">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ36">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -6681,17 +6680,17 @@
         <v>521.8431844622902</v>
       </c>
       <c r="AX37">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY37">
         <v>0</v>
       </c>
       <c r="AZ37">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>88</v>
       </c>
       <c r="B38">
@@ -6836,16 +6835,16 @@
         <v>4164.45</v>
       </c>
       <c r="AX38">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY38">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ38">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -7146,16 +7145,16 @@
         <v>8624.043131856055</v>
       </c>
       <c r="AX40">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY40">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ40">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -7307,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -7453,17 +7452,17 @@
         <v>74.59506853768265</v>
       </c>
       <c r="AX42">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY42">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ42">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>93</v>
       </c>
       <c r="B43">
@@ -7608,16 +7607,16 @@
         <v>106.6253432095332</v>
       </c>
       <c r="AX43">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY43">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ43">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -7763,16 +7762,16 @@
         <v>163.8089263502319</v>
       </c>
       <c r="AX44">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY44">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ44">
-        <v>83.333333333333343</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -7918,16 +7917,16 @@
         <v>1780.869927836208</v>
       </c>
       <c r="AX45">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY45">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ45">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -8079,165 +8078,165 @@
         <v>0</v>
       </c>
       <c r="AZ46">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>3691.42</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>6285.33</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>6063.56</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>8135.66</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>7006.91</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>5925.37</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="2">
         <v>5782.46</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="2">
         <v>7</v>
       </c>
-      <c r="J47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
+      <c r="J47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
+      <c r="L47" s="2">
         <v>6127.244285714286</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="2">
         <v>6.0299999999999999E-2</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="2">
         <v>-0.27710000000000001</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="2">
         <v>47.684091794763837</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="2">
         <v>6127.244285714286</v>
       </c>
-      <c r="R47">
+      <c r="R47" s="2">
         <v>1513.180444753094</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="2">
         <v>6127.244285714286</v>
       </c>
-      <c r="T47">
+      <c r="T47" s="2">
         <v>6184.708333333333</v>
       </c>
-      <c r="U47">
+      <c r="U47" s="2">
         <v>6127.244285714286</v>
       </c>
-      <c r="V47">
+      <c r="V47" s="2">
         <v>-402.24833333333299</v>
       </c>
-      <c r="W47">
+      <c r="W47" s="2">
         <v>-6.5039175924491127E-2</v>
       </c>
-      <c r="X47">
+      <c r="X47" s="2">
         <v>-0.22061483450996919</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Y47" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="AA47" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AB47" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AC47" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AD47" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AE47" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AF47">
+      <c r="AF47" s="2">
         <v>232.0196428571428</v>
       </c>
-      <c r="AG47">
+      <c r="AG47" s="2">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH47" t="s">
+      <c r="AH47" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="AI47" t="s">
+      <c r="AI47" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="AJ47">
+      <c r="AJ47" s="2">
         <v>69</v>
       </c>
-      <c r="AK47">
+      <c r="AK47" s="2">
         <v>5782.46</v>
       </c>
-      <c r="AL47">
+      <c r="AL47" s="2">
         <v>1513.180444753094</v>
       </c>
-      <c r="AM47">
+      <c r="AM47" s="2">
         <v>4269.2795552469061</v>
       </c>
-      <c r="AN47">
+      <c r="AN47" s="2">
         <v>282.13948772933861</v>
       </c>
-      <c r="AO47">
+      <c r="AO47" s="2">
         <v>6184.708333333333</v>
       </c>
-      <c r="AP47">
+      <c r="AP47" s="2">
         <v>13</v>
       </c>
-      <c r="AQ47">
+      <c r="AQ47" s="2">
         <v>3102.269936927813</v>
       </c>
-      <c r="AR47">
-        <v>0</v>
-      </c>
-      <c r="AS47">
+      <c r="AR47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS47" s="2">
         <v>1643.0615210860301</v>
       </c>
-      <c r="AT47">
+      <c r="AT47" s="2">
         <v>2097.8852550436141</v>
       </c>
-      <c r="AU47">
-        <v>0</v>
-      </c>
-      <c r="AV47">
-        <v>0</v>
-      </c>
-      <c r="AW47">
+      <c r="AU47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW47" s="2">
         <v>6843.2167130574562</v>
       </c>
-      <c r="AX47">
-        <v>50</v>
-      </c>
-      <c r="AY47">
-        <v>33.333333333333329</v>
-      </c>
-      <c r="AZ47">
-        <v>66.666666666666657</v>
+      <c r="AX47" s="2">
+        <v>3</v>
+      </c>
+      <c r="AY47" s="2">
+        <v>2</v>
+      </c>
+      <c r="AZ47" s="2">
+        <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -8383,16 +8382,16 @@
         <v>2856.1399929250279</v>
       </c>
       <c r="AX48">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY48">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ48">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -8544,7 +8543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -8696,7 +8695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -8842,16 +8841,16 @@
         <v>1642.314968123133</v>
       </c>
       <c r="AX51">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
       <c r="AY51">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ51">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -8997,16 +8996,16 @@
         <v>2654.9249854207419</v>
       </c>
       <c r="AX52">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY52">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ52">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -9152,16 +9151,16 @@
         <v>3525.5520325123512</v>
       </c>
       <c r="AX53">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY53">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ53">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -9307,16 +9306,16 @@
         <v>79.32079892826431</v>
       </c>
       <c r="AX54">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY54">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -9462,16 +9461,16 @@
         <v>200.62837673741129</v>
       </c>
       <c r="AX55">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY55">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ55">
-        <v>66.666666666666657</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -9623,7 +9622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -9769,16 +9768,16 @@
         <v>5.1400000000000006</v>
       </c>
       <c r="AX57">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY57">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -9924,16 +9923,16 @@
         <v>100.13</v>
       </c>
       <c r="AX58">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY58">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -10079,16 +10078,16 @@
         <v>666.67</v>
       </c>
       <c r="AX59">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY59">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -10231,16 +10230,16 @@
         <v>264.56</v>
       </c>
       <c r="AX60">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY60">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -10386,16 +10385,16 @@
         <v>9144.2793476084116</v>
       </c>
       <c r="AX61">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY61">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ61">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -10544,16 +10543,16 @@
         <v>8946.642365842421</v>
       </c>
       <c r="AX62">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY62">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ62">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>113</v>
       </c>
@@ -10699,16 +10698,16 @@
         <v>3581.8884646499341</v>
       </c>
       <c r="AX63">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY63">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ63">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>114</v>
       </c>
@@ -10854,16 +10853,16 @@
         <v>166.89356973815251</v>
       </c>
       <c r="AX64">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY64">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ64">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>115</v>
       </c>
@@ -11015,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -11161,16 +11160,16 @@
         <v>1146.399747481855</v>
       </c>
       <c r="AX66">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY66">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AZ66">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>117</v>
       </c>
@@ -11322,7 +11321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>118</v>
       </c>
@@ -11474,7 +11473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>119</v>
       </c>
@@ -11626,7 +11625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>120</v>
       </c>
@@ -11778,7 +11777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>121</v>
       </c>
@@ -11933,7 +11932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>122</v>
       </c>
@@ -12091,8 +12090,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>123</v>
       </c>
       <c r="B73">
@@ -12246,7 +12245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>124</v>
       </c>
@@ -12392,16 +12391,16 @@
         <v>5502.7996544406506</v>
       </c>
       <c r="AX74">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY74">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ74">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>125</v>
       </c>
@@ -12547,16 +12546,16 @@
         <v>5627.7996544406506</v>
       </c>
       <c r="AX75">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="AY75">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ75">
-        <v>33.333333333333329</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>126</v>
       </c>
@@ -12708,7 +12707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>127</v>
       </c>
@@ -12854,16 +12853,16 @@
         <v>302.49</v>
       </c>
       <c r="AX77">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY77">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -13009,16 +13008,16 @@
         <v>105.77</v>
       </c>
       <c r="AX78">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY78">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -13164,16 +13163,16 @@
         <v>1596.83</v>
       </c>
       <c r="AX79">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY79">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>130</v>
       </c>
@@ -13319,16 +13318,16 @@
         <v>2005.09</v>
       </c>
       <c r="AX80">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AY80">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
       <c r="AZ80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>131</v>
       </c>
@@ -13480,7 +13479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>132</v>
       </c>
@@ -13626,16 +13625,16 @@
         <v>175349.94970783431</v>
       </c>
       <c r="AX82">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AY82">
         <v>0</v>
       </c>
       <c r="AZ82">
-        <v>16.666666666666661</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>133</v>
       </c>
@@ -13787,7 +13786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>134</v>
       </c>
@@ -13942,7 +13941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>135</v>
       </c>
@@ -14097,7 +14096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>136</v>
       </c>
@@ -14253,14 +14252,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AZ86" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="614200 Internet &amp; Social media"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Profit per Visit percentage above table to match table value and make all percentage values above table show as whole numbers
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16460BC0-57D5-AE47-BFD7-DB7D0EB9F925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EDAFBE-7EE3-3242-902E-53E75FC3B089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="900" windowWidth="25800" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="900" windowWidth="25800" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,12 +709,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -744,11 +756,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="BH1" sqref="BH1"/>
+    <sheetView tabSelected="1" topLeftCell="BQ36" workbookViewId="0">
+      <selection activeCell="BV52" sqref="BV52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4014,227 +4028,227 @@
         <v>-23.311395912712161</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>34271.339999999997</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>36800.629999999997</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>34840.75</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>32894</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>45882.2</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>29065.22</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>28972.19</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>7</v>
       </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
+      <c r="J14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
         <v>34675.19</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="2">
         <v>0.83379999999999999</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="2">
         <v>-0.6048</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="2">
         <v>500.63840187897591</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="2">
         <v>34675.19</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="2">
         <v>8563.3633946065784</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="2">
         <v>34675.19</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="2">
         <v>35625.69</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="2">
         <v>34675.19</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="2">
         <v>-6653.4999999999964</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="2">
         <v>-0.18676129500930361</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="2">
         <v>-0.63349991148688478</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Y14" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB14" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AC14" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AE14" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AF14">
+      <c r="AF14" s="2">
         <v>-725.9578571428566</v>
       </c>
-      <c r="AG14">
+      <c r="AG14" s="2">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AH14" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="2">
         <v>85</v>
       </c>
-      <c r="AK14">
+      <c r="AK14" s="2">
         <v>28972.19</v>
       </c>
-      <c r="AL14">
+      <c r="AL14" s="2">
         <v>8563.3633946065784</v>
       </c>
-      <c r="AM14">
+      <c r="AM14" s="2">
         <v>20408.82660539342</v>
       </c>
-      <c r="AN14">
+      <c r="AN14" s="2">
         <v>238.3272280404147</v>
       </c>
-      <c r="AO14">
+      <c r="AO14" s="2">
         <v>35625.69</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" s="2">
         <v>3</v>
       </c>
-      <c r="AQ14">
+      <c r="AQ14" s="2">
         <v>7248.9307455211347</v>
       </c>
-      <c r="AR14">
-        <v>0</v>
-      </c>
-      <c r="AS14">
-        <v>0</v>
-      </c>
-      <c r="AT14">
+      <c r="AR14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="2">
         <v>26034.091799731628</v>
       </c>
-      <c r="AU14">
-        <v>0</v>
-      </c>
-      <c r="AV14">
-        <v>0</v>
-      </c>
-      <c r="AW14">
+      <c r="AU14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="2">
         <v>-18.771392497407849</v>
       </c>
-      <c r="AX14">
+      <c r="AX14" s="2">
         <v>25.12935401237554</v>
       </c>
-      <c r="AY14">
+      <c r="AY14" s="2">
         <v>2.075686212620468</v>
       </c>
-      <c r="AZ14">
+      <c r="AZ14" s="2">
         <v>-44.660399464132162</v>
       </c>
-      <c r="BA14">
+      <c r="BA14" s="2">
         <v>69.704029999240731</v>
       </c>
-      <c r="BB14">
+      <c r="BB14" s="2">
         <v>19.9253161899384</v>
       </c>
-      <c r="BC14">
+      <c r="BC14" s="2">
         <v>33283.022545252767</v>
       </c>
-      <c r="BD14">
+      <c r="BD14" s="2">
         <v>2</v>
       </c>
-      <c r="BE14">
+      <c r="BE14" s="2">
         <v>2</v>
       </c>
-      <c r="BF14">
+      <c r="BF14" s="2">
         <v>6</v>
       </c>
-      <c r="BG14" t="s">
+      <c r="BG14" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="BH14" t="s">
+      <c r="BH14" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="BI14" t="s">
+      <c r="BI14" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="BJ14">
+      <c r="BJ14" s="2">
         <v>7.3801899779816047</v>
       </c>
-      <c r="BK14">
+      <c r="BK14" s="2">
         <v>-5.3256696964155168</v>
       </c>
-      <c r="BL14">
+      <c r="BL14" s="2">
         <v>-5.587566283733846</v>
       </c>
-      <c r="BM14">
+      <c r="BM14" s="2">
         <v>39.485012464279187</v>
       </c>
-      <c r="BN14">
+      <c r="BN14" s="2">
         <v>-36.652514482740578</v>
       </c>
-      <c r="BO14">
+      <c r="BO14" s="2">
         <v>-0.3200732697017345</v>
       </c>
-      <c r="BP14">
+      <c r="BP14" s="2">
         <v>26.15158247538945</v>
       </c>
-      <c r="BQ14">
+      <c r="BQ14" s="2">
         <v>-30.45502370879105</v>
       </c>
-      <c r="BR14">
+      <c r="BR14" s="2">
         <v>-7.663252496354314</v>
       </c>
-      <c r="BS14">
+      <c r="BS14" s="2">
         <v>84.145411928411349</v>
       </c>
-      <c r="BT14">
+      <c r="BT14" s="2">
         <v>-106.3565444819813</v>
       </c>
-      <c r="BU14">
+      <c r="BU14" s="2">
         <v>-20.24538945964014</v>
       </c>
-      <c r="BV14">
+      <c r="BV14" s="2">
         <v>29.48087152387394</v>
       </c>
-      <c r="BW14">
+      <c r="BW14" s="2">
         <v>-18.676129500930362</v>
       </c>
     </row>
@@ -10880,227 +10894,227 @@
         <v>19.523292997309358</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:75" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>5998.14</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="3">
         <v>2512.91</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="3">
         <v>4456.1000000000004</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <v>2741.61</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>2249.08</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>1783.93</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="3">
         <v>2033</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="3">
         <v>7</v>
       </c>
-      <c r="J45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
+      <c r="J45" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
         <v>3110.681428571429</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="3">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="3">
         <v>0.36890000000000001</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="3">
         <v>-1425.9402149234959</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="3">
         <v>3110.681428571429</v>
       </c>
-      <c r="R45">
+      <c r="R45" s="3">
         <v>768.21195436019445</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="3">
         <v>3110.681428571429</v>
       </c>
-      <c r="T45">
+      <c r="T45" s="3">
         <v>3290.2950000000001</v>
       </c>
-      <c r="U45">
+      <c r="U45" s="3">
         <v>3110.681428571429</v>
       </c>
-      <c r="V45">
+      <c r="V45" s="3">
         <v>-1257.2950000000001</v>
       </c>
-      <c r="W45">
+      <c r="W45" s="3">
         <v>-0.38212227171119922</v>
       </c>
-      <c r="X45">
+      <c r="X45" s="3">
         <v>-1.2961702010802241</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Y45" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="AA45" t="s">
+      <c r="AA45" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="AB45" t="s">
+      <c r="AB45" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="AC45" t="s">
+      <c r="AC45" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AD45" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AE45" t="s">
+      <c r="AE45" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AF45">
+      <c r="AF45" s="3">
         <v>-555.7285714285714</v>
       </c>
-      <c r="AG45">
+      <c r="AG45" s="3">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH45" t="s">
+      <c r="AH45" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AI45" t="s">
+      <c r="AI45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AJ45">
+      <c r="AJ45" s="3">
         <v>78</v>
       </c>
-      <c r="AK45">
+      <c r="AK45" s="3">
         <v>2033</v>
       </c>
-      <c r="AL45">
+      <c r="AL45" s="3">
         <v>768.21195436019445</v>
       </c>
-      <c r="AM45">
+      <c r="AM45" s="3">
         <v>1264.7880456398059</v>
       </c>
-      <c r="AN45">
+      <c r="AN45" s="3">
         <v>164.6405055871833</v>
       </c>
-      <c r="AO45">
+      <c r="AO45" s="3">
         <v>3290.2950000000001</v>
       </c>
-      <c r="AP45">
+      <c r="AP45" s="3">
         <v>24</v>
       </c>
-      <c r="AQ45">
-        <v>0</v>
-      </c>
-      <c r="AR45">
+      <c r="AQ45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR45" s="3">
         <v>1186.0664500876151</v>
       </c>
-      <c r="AS45">
-        <v>0</v>
-      </c>
-      <c r="AT45">
+      <c r="AS45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="3">
         <v>594.80347774859342</v>
       </c>
-      <c r="AU45">
-        <v>0</v>
-      </c>
-      <c r="AV45">
-        <v>0</v>
-      </c>
-      <c r="AW45">
+      <c r="AU45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW45" s="3">
         <v>-18.771392497407849</v>
       </c>
-      <c r="AX45">
+      <c r="AX45" s="3">
         <v>25.12935401237554</v>
       </c>
-      <c r="AY45">
+      <c r="AY45" s="3">
         <v>2.075686212620468</v>
       </c>
-      <c r="AZ45">
+      <c r="AZ45" s="3">
         <v>-44.660399464132162</v>
       </c>
-      <c r="BA45">
+      <c r="BA45" s="3">
         <v>69.704029999240731</v>
       </c>
-      <c r="BB45">
+      <c r="BB45" s="3">
         <v>19.9253161899384</v>
       </c>
-      <c r="BC45">
+      <c r="BC45" s="3">
         <v>1780.869927836208</v>
       </c>
-      <c r="BD45">
+      <c r="BD45" s="3">
         <v>2</v>
       </c>
-      <c r="BE45">
+      <c r="BE45" s="3">
         <v>1</v>
       </c>
-      <c r="BF45">
+      <c r="BF45" s="3">
         <v>2</v>
       </c>
-      <c r="BG45" t="s">
+      <c r="BG45" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="BH45" t="s">
+      <c r="BH45" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="BI45" t="s">
+      <c r="BI45" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="BJ45">
+      <c r="BJ45" s="3">
         <v>-58.105179272241067</v>
       </c>
-      <c r="BK45">
+      <c r="BK45" s="3">
         <v>77.328276778714738</v>
       </c>
-      <c r="BL45">
+      <c r="BL45" s="3">
         <v>-38.475123987343203</v>
       </c>
-      <c r="BM45">
+      <c r="BM45" s="3">
         <v>-17.96499137368189</v>
       </c>
-      <c r="BN45">
+      <c r="BN45" s="3">
         <v>-20.681789887420631</v>
       </c>
-      <c r="BO45">
+      <c r="BO45" s="3">
         <v>13.96187070120464</v>
       </c>
-      <c r="BP45">
+      <c r="BP45" s="3">
         <v>-39.333786774833207</v>
       </c>
-      <c r="BQ45">
+      <c r="BQ45" s="3">
         <v>52.198922766339201</v>
       </c>
-      <c r="BR45">
+      <c r="BR45" s="3">
         <v>-40.550810199963657</v>
       </c>
-      <c r="BS45">
+      <c r="BS45" s="3">
         <v>26.695408090450272</v>
       </c>
-      <c r="BT45">
+      <c r="BT45" s="3">
         <v>-90.385819886661352</v>
       </c>
-      <c r="BU45">
+      <c r="BU45" s="3">
         <v>-5.9634454887337629</v>
       </c>
-      <c r="BV45">
+      <c r="BV45" s="3">
         <v>29.48087152387394</v>
       </c>
-      <c r="BW45">
+      <c r="BW45" s="3">
         <v>-38.21222717111992</v>
       </c>
     </row>
@@ -11322,227 +11336,227 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:75" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="3">
         <v>3691.42</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="3">
         <v>6285.33</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="3">
         <v>6063.56</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="3">
         <v>8135.66</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>7006.91</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>5925.37</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="3">
         <v>5782.46</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="3">
         <v>7</v>
       </c>
-      <c r="J47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
+      <c r="J47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
         <v>6127.244285714286</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="3">
         <v>6.0299999999999999E-2</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="3">
         <v>-0.27710000000000001</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="3">
         <v>47.684091794763837</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="3">
         <v>6127.244285714286</v>
       </c>
-      <c r="R47">
+      <c r="R47" s="3">
         <v>1513.180444753094</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="3">
         <v>6127.244285714286</v>
       </c>
-      <c r="T47">
+      <c r="T47" s="3">
         <v>6184.708333333333</v>
       </c>
-      <c r="U47">
+      <c r="U47" s="3">
         <v>6127.244285714286</v>
       </c>
-      <c r="V47">
+      <c r="V47" s="3">
         <v>-402.24833333333299</v>
       </c>
-      <c r="W47">
+      <c r="W47" s="3">
         <v>-6.5039175924491127E-2</v>
       </c>
-      <c r="X47">
+      <c r="X47" s="3">
         <v>-0.22061483450996919</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Y47" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="AA47" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AB47" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AC47" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AD47" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AE47" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AF47">
+      <c r="AF47" s="3">
         <v>232.0196428571428</v>
       </c>
-      <c r="AG47">
+      <c r="AG47" s="3">
         <v>1961.3796428571441</v>
       </c>
-      <c r="AH47" t="s">
+      <c r="AH47" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AI47" t="s">
+      <c r="AI47" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AJ47">
+      <c r="AJ47" s="3">
         <v>69</v>
       </c>
-      <c r="AK47">
+      <c r="AK47" s="3">
         <v>5782.46</v>
       </c>
-      <c r="AL47">
+      <c r="AL47" s="3">
         <v>1513.180444753094</v>
       </c>
-      <c r="AM47">
+      <c r="AM47" s="3">
         <v>4269.2795552469061</v>
       </c>
-      <c r="AN47">
+      <c r="AN47" s="3">
         <v>282.13948772933861</v>
       </c>
-      <c r="AO47">
+      <c r="AO47" s="3">
         <v>6184.708333333333</v>
       </c>
-      <c r="AP47">
+      <c r="AP47" s="3">
         <v>13</v>
       </c>
-      <c r="AQ47">
+      <c r="AQ47" s="3">
         <v>3102.269936927813</v>
       </c>
-      <c r="AR47">
-        <v>0</v>
-      </c>
-      <c r="AS47">
+      <c r="AR47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS47" s="3">
         <v>1643.0615210860301</v>
       </c>
-      <c r="AT47">
+      <c r="AT47" s="3">
         <v>2097.8852550436141</v>
       </c>
-      <c r="AU47">
-        <v>0</v>
-      </c>
-      <c r="AV47">
-        <v>0</v>
-      </c>
-      <c r="AW47">
+      <c r="AU47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW47" s="3">
         <v>-18.771392497407849</v>
       </c>
-      <c r="AX47">
+      <c r="AX47" s="3">
         <v>25.12935401237554</v>
       </c>
-      <c r="AY47">
+      <c r="AY47" s="3">
         <v>2.075686212620468</v>
       </c>
-      <c r="AZ47">
+      <c r="AZ47" s="3">
         <v>-44.660399464132162</v>
       </c>
-      <c r="BA47">
+      <c r="BA47" s="3">
         <v>69.704029999240731</v>
       </c>
-      <c r="BB47">
+      <c r="BB47" s="3">
         <v>19.9253161899384</v>
       </c>
-      <c r="BC47">
+      <c r="BC47" s="3">
         <v>6843.2167130574562</v>
       </c>
-      <c r="BD47">
+      <c r="BD47" s="3">
         <v>3</v>
       </c>
-      <c r="BE47">
+      <c r="BE47" s="3">
         <v>2</v>
       </c>
-      <c r="BF47">
+      <c r="BF47" s="3">
         <v>4</v>
       </c>
-      <c r="BG47" t="s">
+      <c r="BG47" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="BH47" t="s">
+      <c r="BH47" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="BI47" t="s">
+      <c r="BI47" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="BJ47">
+      <c r="BJ47" s="3">
         <v>70.268622914759078</v>
       </c>
-      <c r="BK47">
+      <c r="BK47" s="3">
         <v>-3.52837480291408</v>
       </c>
-      <c r="BL47">
+      <c r="BL47" s="3">
         <v>34.172994082684092</v>
       </c>
-      <c r="BM47">
+      <c r="BM47" s="3">
         <v>-13.874104866722551</v>
       </c>
-      <c r="BN47">
+      <c r="BN47" s="3">
         <v>-15.435334548324439</v>
       </c>
-      <c r="BO47">
+      <c r="BO47" s="3">
         <v>-2.4118325100373461</v>
       </c>
-      <c r="BP47">
+      <c r="BP47" s="3">
         <v>89.040015412166923</v>
       </c>
-      <c r="BQ47">
+      <c r="BQ47" s="3">
         <v>-28.657728815289619</v>
       </c>
-      <c r="BR47">
+      <c r="BR47" s="3">
         <v>32.097307870063617</v>
       </c>
-      <c r="BS47">
+      <c r="BS47" s="3">
         <v>30.786294597409611</v>
       </c>
-      <c r="BT47">
+      <c r="BT47" s="3">
         <v>-85.139364547565165</v>
       </c>
-      <c r="BU47">
+      <c r="BU47" s="3">
         <v>-22.337148699975749</v>
       </c>
-      <c r="BV47">
+      <c r="BV47" s="3">
         <v>29.48087152387394</v>
       </c>
-      <c r="BW47">
+      <c r="BW47" s="3">
         <v>-6.5039175924491124</v>
       </c>
     </row>

</xml_diff>